<commit_message>
`Removed demo credentials from LoginPage.js`
</commit_message>
<xml_diff>
--- a/student-attendance/scripts/Teachers/Teachers Data.xlsx
+++ b/student-attendance/scripts/Teachers/Teachers Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7642D7F-B554-4531-80C5-7C7E05ADDCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D57C1A8-3DB1-4E58-98B1-F397162F35FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="23" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGRI" sheetId="3" r:id="rId1"/>
@@ -1472,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I389"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2183,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB97ECA-1649-E747-B272-90EDD1CF5DB3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2495,8 +2495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058C218E-3F62-714F-B6A8-C2BDDECA3C9D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4307,7 +4307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E34F051-D216-0C45-BB9B-9D364F9DDA85}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4458,7 +4458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BA9AD2-5A9F-AE46-95B4-DD5F8DC75C96}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -4620,7 +4620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F926895-4B62-5A4A-8075-D22E29868675}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -4770,7 +4770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB76736E-9181-4C44-BC6F-B0E73EB602F5}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -5683,8 +5683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8C2DE1-6397-784A-8525-25ADCE04E819}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>75</v>
@@ -5845,7 +5845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B840F4-7383-0F40-96E9-5A319E87D85A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -6298,7 +6298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A208E9B9-A03E-EE43-ACDA-72DC262B5D31}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -6449,7 +6449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57934096-E133-CC48-8019-7834699460B9}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -6600,7 +6600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D2E2C5-61C1-514E-BA68-ED08D4A83B52}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
`Updated seedAttendance20260206.js to use attendance date 2026-02-09 instead of 2026-02-08`
</commit_message>
<xml_diff>
--- a/student-attendance/scripts/Teachers/Teachers Data.xlsx
+++ b/student-attendance/scripts/Teachers/Teachers Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D57C1A8-3DB1-4E58-98B1-F397162F35FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0659B3-0FC9-4265-88CB-001FA351EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="23" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="16680" windowHeight="13056" firstSheet="26" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGRI" sheetId="3" r:id="rId1"/>
@@ -747,9 +747,6 @@
     <t>G.Deivamani (9894828429)</t>
   </si>
   <si>
-    <t>M.Tamilselvi (8508069523)</t>
-  </si>
-  <si>
     <t>C.Manjula (8220532395)</t>
   </si>
   <si>
@@ -816,9 +813,6 @@
     <t xml:space="preserve">G.Visalakshi (6374058052) </t>
   </si>
   <si>
-    <t>S.Satheesh Kumar (87788517744)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A.Meignanamoorthi (9789424652) </t>
   </si>
   <si>
@@ -903,9 +897,6 @@
     <t xml:space="preserve">Monisha (6385642716) </t>
   </si>
   <si>
-    <t>A.Priyadharshini ( 90254 27989)</t>
-  </si>
-  <si>
     <t xml:space="preserve">S.Thirunavukkarasu (9790079420) </t>
   </si>
   <si>
@@ -924,16 +915,25 @@
     <t xml:space="preserve">A.Jayapal (8754807710) </t>
   </si>
   <si>
-    <t>Hahadevan (3333333333)</t>
-  </si>
-  <si>
-    <t>Hemalatha (4444444444)</t>
-  </si>
-  <si>
     <t xml:space="preserve">N.Satheeshwaran (8098271534) </t>
   </si>
   <si>
-    <t>Harini (5555555555)</t>
+    <t>A.Priyadharshini (9025427989)</t>
+  </si>
+  <si>
+    <t>S.Satheesh Kumar (7777777777)</t>
+  </si>
+  <si>
+    <t>Harini (6383547455)</t>
+  </si>
+  <si>
+    <t>Mahadevan (6369391484)</t>
+  </si>
+  <si>
+    <t>A.Jeeva (9698444896)</t>
+  </si>
+  <si>
+    <t>Hemalatha (9940826805)</t>
   </si>
 </sst>
 </file>
@@ -1473,7 +1473,7 @@
   <dimension ref="A1:I389"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1510,7 +1510,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1554,7 +1554,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1598,7 +1598,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2146,7 +2146,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -2157,7 +2157,7 @@
         <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2168,7 +2168,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2307,7 @@
         <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2329,7 +2329,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2345,7 +2345,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2425,7 +2425,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2458,7 +2458,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2469,7 +2469,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2496,7 +2496,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2532,7 +2532,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2576,7 +2576,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2609,7 +2609,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2620,7 +2620,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2646,7 +2646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950A2374-A4F1-B048-BBBA-060C90169EDE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2727,7 +2727,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2760,7 +2760,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2771,7 +2771,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2911,7 +2911,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3062,7 +3062,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3084,7 +3084,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3100,7 +3100,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,7 +3158,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3213,7 +3213,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3235,7 +3235,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3251,7 +3251,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3320,7 +3320,7 @@
         <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3364,7 +3364,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3375,7 +3375,7 @@
         <v>55</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3397,7 +3397,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3449,7 +3449,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3526,7 +3526,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3548,7 +3548,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3677,7 +3677,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3699,7 +3699,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3762,7 +3762,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3828,7 +3828,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>231</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3855,7 +3855,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3935,7 +3935,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3979,7 +3979,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3990,7 +3990,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4006,7 +4006,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4042,7 +4042,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4130,7 +4130,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4141,7 +4141,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4157,7 +4157,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4237,7 +4237,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>208</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4270,7 +4270,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4281,7 +4281,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4292,7 +4292,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4344,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4355,7 +4355,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4377,7 +4377,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4399,7 +4399,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4421,7 +4421,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4443,7 +4443,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4459,7 +4459,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4506,7 +4506,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4528,7 +4528,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4539,7 +4539,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4572,7 +4572,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4583,7 +4583,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4594,7 +4594,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4605,7 +4605,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4621,7 +4621,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4667,7 +4667,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4700,7 +4700,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4733,7 +4733,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4755,7 +4755,7 @@
         <v>92</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4807,7 +4807,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4818,7 +4818,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4851,7 +4851,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4862,7 +4862,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4884,7 +4884,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4906,7 +4906,7 @@
         <v>92</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4922,7 +4922,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4969,7 +4969,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4991,7 +4991,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5002,7 +5002,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5035,7 +5035,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5046,7 +5046,7 @@
         <v>116</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5057,7 +5057,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5073,7 +5073,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5120,7 +5120,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5131,7 +5131,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5142,7 +5142,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5153,7 +5153,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5164,7 +5164,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5175,7 +5175,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5186,7 +5186,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5208,7 +5208,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5440,7 +5440,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5484,7 +5484,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5495,7 +5495,7 @@
         <v>102</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5522,7 +5522,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5569,7 +5569,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5591,7 +5591,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5613,7 +5613,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5646,7 +5646,7 @@
         <v>116</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5668,7 +5668,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5753,7 +5753,7 @@
         <v>112</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5797,7 +5797,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5808,7 +5808,7 @@
         <v>114</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5959,7 +5959,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5981,7 +5981,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -6110,7 +6110,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -6132,7 +6132,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -6261,7 +6261,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -6283,7 +6283,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -6412,7 +6412,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -6434,7 +6434,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -6486,7 +6486,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -6563,7 +6563,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -6714,7 +6714,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -6736,7 +6736,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Updated AdminDashboard component to include S.No column in teacher list`
</commit_message>
<xml_diff>
--- a/student-attendance/scripts/Teachers/Teachers Data.xlsx
+++ b/student-attendance/scripts/Teachers/Teachers Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0659B3-0FC9-4265-88CB-001FA351EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9816C97-5F6A-4F08-9E04-A3C3439F2F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="16680" windowHeight="13056" firstSheet="26" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="17" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGRI" sheetId="3" r:id="rId1"/>
@@ -921,9 +921,6 @@
     <t>A.Priyadharshini (9025427989)</t>
   </si>
   <si>
-    <t>S.Satheesh Kumar (7777777777)</t>
-  </si>
-  <si>
     <t>Harini (6383547455)</t>
   </si>
   <si>
@@ -934,6 +931,9 @@
   </si>
   <si>
     <t>Hemalatha (9940826805)</t>
+  </si>
+  <si>
+    <t>R.Satheesh Kumar (9500593108)</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1554,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1598,7 +1598,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2425,7 +2425,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2469,7 +2469,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2576,7 +2576,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2620,7 +2620,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2727,7 +2727,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -2771,7 +2771,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3158,7 +3158,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3320,7 +3320,7 @@
         <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -3364,7 +3364,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3714,7 +3714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA559E0-6D60-4B46-831C-0C87556BAE85}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3828,7 +3828,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3935,7 +3935,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -3979,7 +3979,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4130,7 +4130,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4237,7 +4237,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4281,7 +4281,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -4528,7 +4528,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4583,7 +4583,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5073,7 +5073,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5131,7 +5131,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -5175,7 +5175,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -5683,7 +5683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8C2DE1-6397-784A-8525-25ADCE04E819}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>